<commit_message>
Write csv of monitoring events with PRISM data
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/03.2_monitoring-events-with-Farrell-climate-data-and-PRISM-csv-file-name.xlsx
+++ b/data/data-wrangling-intermediate/03.2_monitoring-events-with-Farrell-climate-data-and-PRISM-csv-file-name.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="697" documentId="8_{183721BE-512D-4019-AD76-4D99915CCEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{510B716F-EE01-4044-A9FD-1D5C13067982}"/>
+  <xr:revisionPtr revIDLastSave="704" documentId="8_{183721BE-512D-4019-AD76-4D99915CCEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B8B6B8A-B13E-486D-87C3-7C1279DAA33C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B4335E2B-D23C-409E-810D-4935D7243195}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="435">
   <si>
     <t>Region</t>
   </si>
@@ -1973,10 +1973,10 @@
   <dimension ref="A1:Q191"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E176" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O190" activeCellId="20" sqref="O2 O11 O17 O25 O44 O57 O74 O86 O102 O111 O116 O121 O124 O131 O137 O141 O144 O158 O169 O179 O190"/>
+      <selection pane="bottomRight" activeCell="H114" activeCellId="20" sqref="H5:I5 H9:I9 H15:I15 H25:I25 H42:I42 H58:I58 H74:I74 H82:I82 H99:I99 H112:I112 H118:I118 H123:I123 H129:I129 H134:I134 H139:I139 H143:I143 H154:I154 H165:I165 H178:I178 H187:I187 H114:I114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10837,10 +10837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2026BC2C-D6E3-4854-AE76-7746F280B3CE}">
-  <dimension ref="A1:I146"/>
+  <dimension ref="A1:K146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10848,13 +10848,13 @@
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.21875" customWidth="1"/>
     <col min="3" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10871,19 +10871,25 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>140</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -10899,20 +10905,26 @@
       <c r="E2">
         <v>4484</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2">
         <v>296.5</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>16.2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>141</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -10928,20 +10940,26 @@
       <c r="E3">
         <v>4327</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
         <v>274.76</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>15.7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>142</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -10957,20 +10975,26 @@
       <c r="E4">
         <v>3300</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
         <v>455.05</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>18.5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>143</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -10986,20 +11010,26 @@
       <c r="E5">
         <v>6473</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5">
         <v>516.16</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>9.5</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>144</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -11015,20 +11045,26 @@
       <c r="E6">
         <v>5603</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6">
         <v>311.02</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>11</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>145</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -11044,20 +11080,26 @@
       <c r="E7">
         <v>5226</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7">
         <v>358.85</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>10.6</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>146</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -11073,20 +11115,26 @@
       <c r="E8">
         <v>3522</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8">
         <v>383.29</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>16.3</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>147</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -11102,20 +11150,26 @@
       <c r="E9">
         <v>5386</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9">
         <v>243.62</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>12.6</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>148</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -11131,20 +11185,26 @@
       <c r="E10">
         <v>5226</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10">
         <v>171.4</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>13.2</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>149</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -11160,20 +11220,26 @@
       <c r="E11">
         <v>4914</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11">
         <v>179.73</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>13</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>150</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -11189,20 +11255,26 @@
       <c r="E12">
         <v>1935</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12">
         <v>97.61</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>19.7</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>151</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -11218,20 +11290,26 @@
       <c r="E13">
         <v>2467</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13">
         <v>221.63</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>16.7</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>152</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -11247,20 +11325,26 @@
       <c r="E14">
         <v>1771</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14">
         <v>310.94</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>21.3</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
         <v>153</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -11276,20 +11360,26 @@
       <c r="E15">
         <v>2621</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15">
         <v>371.13</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>20.7</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>154</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -11305,20 +11395,26 @@
       <c r="E16">
         <v>2500</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16">
         <v>417.48</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>19.899999999999999</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" t="s">
         <v>155</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -11334,20 +11430,26 @@
       <c r="E17">
         <v>1263</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17">
         <v>245.02</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>22.4</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>156</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -11363,20 +11465,26 @@
       <c r="E18">
         <v>4331</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18">
         <v>485.89</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>16.5</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
         <v>157</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -11392,20 +11500,26 @@
       <c r="E19">
         <v>3868</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19">
         <v>534.92999999999995</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>17.899999999999999</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>158</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -11421,20 +11535,26 @@
       <c r="E20">
         <v>5331</v>
       </c>
-      <c r="F20">
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20">
         <v>224.99</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>12</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>159</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -11450,20 +11570,26 @@
       <c r="E21">
         <v>4724</v>
       </c>
-      <c r="F21">
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21">
         <v>273.55</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>12</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>160</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -11479,16 +11605,22 @@
       <c r="E22">
         <v>7486</v>
       </c>
-      <c r="F22">
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22">
         <v>415.66</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>8.5</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>161</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>434</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Write csv of monthly normals for all sites, and daily values for all sites from 03.2.R. Also start visualizing precip trends in 03.3.R
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/03.2_monitoring-events-with-Farrell-climate-data-and-PRISM-csv-file-name.xlsx
+++ b/data/data-wrangling-intermediate/03.2_monitoring-events-with-Farrell-climate-data-and-PRISM-csv-file-name.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="704" documentId="8_{183721BE-512D-4019-AD76-4D99915CCEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B8B6B8A-B13E-486D-87C3-7C1279DAA33C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B4335E2B-D23C-409E-810D-4935D7243195}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4335E2B-D23C-409E-810D-4935D7243195}"/>
   </bookViews>
   <sheets>
     <sheet name="daily" sheetId="1" r:id="rId1"/>
@@ -1972,11 +1972,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{579BD239-D9C9-473B-862B-ED453983378D}">
   <dimension ref="A1:Q191"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E98" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H114" activeCellId="20" sqref="H5:I5 H9:I9 H15:I15 H25:I25 H42:I42 H58:I58 H74:I74 H82:I82 H99:I99 H112:I112 H118:I118 H123:I123 H129:I129 H134:I134 H139:I139 H143:I143 H154:I154 H165:I165 H178:I178 H187:I187 H114:I114"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10839,7 +10839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2026BC2C-D6E3-4854-AE76-7746F280B3CE}">
   <dimension ref="A1:K146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Reassign SiteDateID because 29 Palms was completely reseeded, so from 115-188 IDs needed to be changed
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/03.2_monitoring-events-with-Farrell-climate-data-and-PRISM-csv-file-name.xlsx
+++ b/data/data-wrangling-intermediate/03.2_monitoring-events-with-Farrell-climate-data-and-PRISM-csv-file-name.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="738" documentId="8_{183721BE-512D-4019-AD76-4D99915CCEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7BE22A5-2C4F-47E2-95FB-FDE026D4AC4C}"/>
+  <xr:revisionPtr revIDLastSave="835" documentId="8_{183721BE-512D-4019-AD76-4D99915CCEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0969104E-1016-4415-ADB2-39979521A934}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B4335E2B-D23C-409E-810D-4935D7243195}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{B4335E2B-D23C-409E-810D-4935D7243195}"/>
   </bookViews>
   <sheets>
     <sheet name="daily" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,10 @@
   <authors>
     <author>tc={E8B8152E-943A-4C86-BED8-BBCAAEFCCFCA}</author>
     <author>tc={D6960D43-F591-4885-B084-821F40E4C2C2}</author>
+    <author>tc={E3896B76-4F91-4A5D-BCD6-98FF14E6F944}</author>
   </authors>
   <commentList>
-    <comment ref="Q147" authorId="0" shapeId="0" xr:uid="{E8B8152E-943A-4C86-BED8-BBCAAEFCCFCA}">
+    <comment ref="Q146" authorId="0" shapeId="0" xr:uid="{E8B8152E-943A-4C86-BED8-BBCAAEFCCFCA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -51,12 +52,20 @@
     Time window is slightly variable and technically plot-specific, but precip and temp are most likely very similar so being plot-specific is not necessary.</t>
       </text>
     </comment>
-    <comment ref="Q156" authorId="1" shapeId="0" xr:uid="{D6960D43-F591-4885-B084-821F40E4C2C2}">
+    <comment ref="Q155" authorId="1" shapeId="0" xr:uid="{D6960D43-F591-4885-B084-821F40E4C2C2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Time window is slightly variable and technically plot-specific, but precip and temp are most likely very similar so being plot-specific is not necessary.</t>
+      </text>
+    </comment>
+    <comment ref="E189" authorId="2" shapeId="0" xr:uid="{E3896B76-4F91-4A5D-BCD6-98FF14E6F944}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I thought some plots weren't reseeded, but it turns out all of them were. However, I still want to save this file because it contains all of the days of the experiment.</t>
       </text>
     </comment>
   </commentList>
@@ -1375,7 +1384,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1389,6 +1398,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1432,7 +1447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1440,8 +1455,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1638,14 +1651,15 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Ossanna, Lia Qin Ryan - (lossanna)" id="{E914B418-0B4D-4548-A199-D322254992A1}" userId="S::lossanna@arizona.edu::4ef914cd-790d-460d-a4af-cca4fc5cf0d2" providerId="AD"/>
   <person displayName="Ossanna, Lia Qin Ryan - (lossanna)" id="{71ACD4BE-3DF0-4830-A25D-EEA83051C07D}" userId="S::lossanna@email.arizona.edu::4ef914cd-790d-460d-a4af-cca4fc5cf0d2" providerId="AD"/>
 </personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1683,7 +1697,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1789,7 +1803,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1931,7 +1945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1939,11 +1953,14 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="Q147" dT="2023-09-27T18:19:27.55" personId="{71ACD4BE-3DF0-4830-A25D-EEA83051C07D}" id="{E8B8152E-943A-4C86-BED8-BBCAAEFCCFCA}">
+  <threadedComment ref="Q146" dT="2023-09-27T18:19:27.55" personId="{71ACD4BE-3DF0-4830-A25D-EEA83051C07D}" id="{E8B8152E-943A-4C86-BED8-BBCAAEFCCFCA}">
     <text>Time window is slightly variable and technically plot-specific, but precip and temp are most likely very similar so being plot-specific is not necessary.</text>
   </threadedComment>
-  <threadedComment ref="Q156" dT="2023-09-27T18:20:11.25" personId="{71ACD4BE-3DF0-4830-A25D-EEA83051C07D}" id="{D6960D43-F591-4885-B084-821F40E4C2C2}">
+  <threadedComment ref="Q155" dT="2023-09-27T18:20:11.25" personId="{71ACD4BE-3DF0-4830-A25D-EEA83051C07D}" id="{D6960D43-F591-4885-B084-821F40E4C2C2}">
     <text>Time window is slightly variable and technically plot-specific, but precip and temp are most likely very similar so being plot-specific is not necessary.</text>
+  </threadedComment>
+  <threadedComment ref="E189" dT="2024-03-04T23:02:28.00" personId="{E914B418-0B4D-4548-A199-D322254992A1}" id="{E3896B76-4F91-4A5D-BCD6-98FF14E6F944}">
+    <text>I thought some plots weren't reseeded, but it turns out all of them were. However, I still want to save this file because it contains all of the days of the experiment.</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1953,10 +1970,10 @@
   <dimension ref="A1:Q189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="L158" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G56" sqref="G56"/>
+      <selection pane="bottomRight" activeCell="E189" sqref="E189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5110,19 +5127,19 @@
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
+      <c r="A64" t="s">
         <v>18</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="8">
+      <c r="C64" s="1">
         <v>44029</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D64" s="1">
         <v>44111</v>
       </c>
-      <c r="E64" s="7">
+      <c r="E64">
         <v>63</v>
       </c>
       <c r="F64">
@@ -7650,29 +7667,56 @@
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A116" s="5" t="s">
+      <c r="A116" t="s">
         <v>27</v>
       </c>
-      <c r="B116" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C116" s="6">
-        <v>43903</v>
-      </c>
-      <c r="D116" s="6">
-        <v>44666</v>
-      </c>
-      <c r="E116" s="5">
+      <c r="B116" t="s">
+        <v>29</v>
+      </c>
+      <c r="C116" s="1">
+        <v>43907</v>
+      </c>
+      <c r="D116" s="1">
+        <v>43951</v>
+      </c>
+      <c r="E116">
         <v>115</v>
       </c>
+      <c r="F116">
+        <v>34.701538999999997</v>
+      </c>
+      <c r="G116">
+        <v>-118.30973400000001</v>
+      </c>
+      <c r="H116">
+        <v>2467</v>
+      </c>
+      <c r="I116" t="s">
+        <v>15</v>
+      </c>
+      <c r="J116" t="s">
+        <v>16</v>
+      </c>
+      <c r="K116">
+        <v>221.63</v>
+      </c>
+      <c r="L116">
+        <v>16.7</v>
+      </c>
+      <c r="M116">
+        <v>85.766000379999994</v>
+      </c>
+      <c r="N116">
+        <v>85.766000379999994</v>
+      </c>
       <c r="O116" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="P116" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="Q116" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
@@ -7686,46 +7730,20 @@
         <v>43907</v>
       </c>
       <c r="D117" s="1">
-        <v>43951</v>
+        <v>44292</v>
       </c>
       <c r="E117">
+        <f>E116+1</f>
         <v>116</v>
-      </c>
-      <c r="F117">
-        <v>34.701538999999997</v>
-      </c>
-      <c r="G117">
-        <v>-118.30973400000001</v>
-      </c>
-      <c r="H117">
-        <v>2467</v>
-      </c>
-      <c r="I117" t="s">
-        <v>15</v>
-      </c>
-      <c r="J117" t="s">
-        <v>16</v>
-      </c>
-      <c r="K117">
-        <v>221.63</v>
-      </c>
-      <c r="L117">
-        <v>16.7</v>
-      </c>
-      <c r="M117">
-        <v>85.766000379999994</v>
-      </c>
-      <c r="N117">
-        <v>85.766000379999994</v>
       </c>
       <c r="O117" t="s">
         <v>151</v>
       </c>
       <c r="P117" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="Q117" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
@@ -7736,22 +7754,23 @@
         <v>29</v>
       </c>
       <c r="C118" s="1">
-        <v>43907</v>
+        <v>44578</v>
       </c>
       <c r="D118" s="1">
-        <v>44292</v>
+        <v>44664</v>
       </c>
       <c r="E118">
+        <f t="shared" ref="E118:E181" si="0">E117+1</f>
         <v>117</v>
       </c>
       <c r="O118" t="s">
         <v>151</v>
       </c>
       <c r="P118" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="Q118" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.3">
@@ -7762,74 +7781,104 @@
         <v>29</v>
       </c>
       <c r="C119" s="1">
-        <v>44578</v>
+        <v>44576</v>
       </c>
       <c r="D119" s="1">
         <v>44664</v>
       </c>
       <c r="E119">
+        <f t="shared" si="0"/>
         <v>118</v>
       </c>
       <c r="O119" t="s">
         <v>151</v>
       </c>
       <c r="P119" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="Q119" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="A120" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C120" s="1">
-        <v>44576</v>
-      </c>
-      <c r="D120" s="1">
+      <c r="C120" s="6">
+        <v>43907</v>
+      </c>
+      <c r="D120" s="6">
         <v>44664</v>
       </c>
-      <c r="E120">
+      <c r="E120" s="5">
+        <f t="shared" si="0"/>
         <v>119</v>
       </c>
       <c r="O120" t="s">
         <v>151</v>
       </c>
       <c r="P120" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Q120" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A121" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C121" s="6">
-        <v>43907</v>
-      </c>
-      <c r="D121" s="6">
-        <v>44664</v>
-      </c>
-      <c r="E121" s="5">
+      <c r="A121" t="s">
+        <v>30</v>
+      </c>
+      <c r="B121" t="s">
+        <v>31</v>
+      </c>
+      <c r="C121" s="1">
+        <v>43818</v>
+      </c>
+      <c r="D121" s="1">
+        <v>43920</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
+      <c r="F121">
+        <v>33.93656</v>
+      </c>
+      <c r="G121">
+        <v>-112.3232</v>
+      </c>
+      <c r="H121">
+        <v>1771</v>
+      </c>
+      <c r="I121" t="s">
+        <v>15</v>
+      </c>
+      <c r="J121" t="s">
+        <v>16</v>
+      </c>
+      <c r="K121">
+        <v>310.94</v>
+      </c>
+      <c r="L121">
+        <v>21.3</v>
+      </c>
+      <c r="M121">
+        <v>193.78299999999999</v>
+      </c>
+      <c r="N121">
+        <v>193.78299999999999</v>
+      </c>
       <c r="O121" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="P121" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="Q121" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.3">
@@ -7843,9 +7892,10 @@
         <v>43818</v>
       </c>
       <c r="D122" s="1">
-        <v>43920</v>
+        <v>44118</v>
       </c>
       <c r="E122">
+        <f t="shared" si="0"/>
         <v>121</v>
       </c>
       <c r="F122">
@@ -7870,19 +7920,19 @@
         <v>21.3</v>
       </c>
       <c r="M122">
-        <v>193.78299999999999</v>
+        <v>226.78399999999999</v>
       </c>
       <c r="N122">
-        <v>193.78299999999999</v>
+        <v>33.783999999999999</v>
       </c>
       <c r="O122" t="s">
         <v>152</v>
       </c>
       <c r="P122" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="Q122" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.3">
@@ -7896,46 +7946,20 @@
         <v>43818</v>
       </c>
       <c r="D123" s="1">
-        <v>44118</v>
+        <v>44288</v>
       </c>
       <c r="E123">
+        <f t="shared" si="0"/>
         <v>122</v>
-      </c>
-      <c r="F123">
-        <v>33.93656</v>
-      </c>
-      <c r="G123">
-        <v>-112.3232</v>
-      </c>
-      <c r="H123">
-        <v>1771</v>
-      </c>
-      <c r="I123" t="s">
-        <v>15</v>
-      </c>
-      <c r="J123" t="s">
-        <v>16</v>
-      </c>
-      <c r="K123">
-        <v>310.94</v>
-      </c>
-      <c r="L123">
-        <v>21.3</v>
-      </c>
-      <c r="M123">
-        <v>226.78399999999999</v>
-      </c>
-      <c r="N123">
-        <v>33.783999999999999</v>
       </c>
       <c r="O123" t="s">
         <v>152</v>
       </c>
       <c r="P123" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="Q123" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.3">
@@ -7949,19 +7973,20 @@
         <v>43818</v>
       </c>
       <c r="D124" s="1">
-        <v>44288</v>
+        <v>44473</v>
       </c>
       <c r="E124">
+        <f t="shared" si="0"/>
         <v>123</v>
       </c>
       <c r="O124" t="s">
         <v>152</v>
       </c>
       <c r="P124" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="Q124" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.3">
@@ -7975,71 +8000,101 @@
         <v>43818</v>
       </c>
       <c r="D125" s="1">
-        <v>44473</v>
+        <v>44649</v>
       </c>
       <c r="E125">
+        <f t="shared" si="0"/>
         <v>124</v>
       </c>
       <c r="O125" t="s">
         <v>152</v>
       </c>
       <c r="P125" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="Q125" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+      <c r="A126" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="6">
         <v>43818</v>
       </c>
-      <c r="D126" s="1">
-        <v>44649</v>
-      </c>
-      <c r="E126">
+      <c r="D126" s="6">
+        <v>45009</v>
+      </c>
+      <c r="E126" s="5">
+        <f t="shared" si="0"/>
         <v>125</v>
       </c>
       <c r="O126" t="s">
         <v>152</v>
       </c>
       <c r="P126" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="Q126" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A127" s="5" t="s">
+      <c r="A127" t="s">
         <v>30</v>
       </c>
-      <c r="B127" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C127" s="6">
-        <v>43818</v>
-      </c>
-      <c r="D127" s="6">
-        <v>45009</v>
-      </c>
-      <c r="E127" s="5">
+      <c r="B127" t="s">
+        <v>32</v>
+      </c>
+      <c r="C127" s="1">
+        <v>43794</v>
+      </c>
+      <c r="D127" s="1">
+        <v>43916</v>
+      </c>
+      <c r="E127">
+        <f t="shared" si="0"/>
         <v>126</v>
       </c>
+      <c r="F127">
+        <v>33.769526999999997</v>
+      </c>
+      <c r="G127">
+        <v>-111.793977</v>
+      </c>
+      <c r="H127">
+        <v>2621</v>
+      </c>
+      <c r="I127" t="s">
+        <v>15</v>
+      </c>
+      <c r="J127" t="s">
+        <v>16</v>
+      </c>
+      <c r="K127">
+        <v>371.13</v>
+      </c>
+      <c r="L127">
+        <v>20.7</v>
+      </c>
+      <c r="M127">
+        <v>236.589</v>
+      </c>
+      <c r="N127">
+        <v>236.589</v>
+      </c>
       <c r="O127" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="P127" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="Q127" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.3">
@@ -8053,9 +8108,10 @@
         <v>43794</v>
       </c>
       <c r="D128" s="1">
-        <v>43916</v>
+        <v>44116</v>
       </c>
       <c r="E128">
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="F128">
@@ -8080,19 +8136,19 @@
         <v>20.7</v>
       </c>
       <c r="M128">
-        <v>236.589</v>
+        <v>263.66199999999998</v>
       </c>
       <c r="N128">
-        <v>236.589</v>
+        <v>27.661999999999999</v>
       </c>
       <c r="O128" t="s">
         <v>153</v>
       </c>
       <c r="P128" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="Q128" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.3">
@@ -8106,46 +8162,20 @@
         <v>43794</v>
       </c>
       <c r="D129" s="1">
-        <v>44116</v>
+        <v>44285</v>
       </c>
       <c r="E129">
+        <f t="shared" si="0"/>
         <v>128</v>
-      </c>
-      <c r="F129">
-        <v>33.769526999999997</v>
-      </c>
-      <c r="G129">
-        <v>-111.793977</v>
-      </c>
-      <c r="H129">
-        <v>2621</v>
-      </c>
-      <c r="I129" t="s">
-        <v>15</v>
-      </c>
-      <c r="J129" t="s">
-        <v>16</v>
-      </c>
-      <c r="K129">
-        <v>371.13</v>
-      </c>
-      <c r="L129">
-        <v>20.7</v>
-      </c>
-      <c r="M129">
-        <v>263.66199999999998</v>
-      </c>
-      <c r="N129">
-        <v>27.661999999999999</v>
       </c>
       <c r="O129" t="s">
         <v>153</v>
       </c>
       <c r="P129" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="Q129" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.3">
@@ -8159,71 +8189,101 @@
         <v>43794</v>
       </c>
       <c r="D130" s="1">
-        <v>44285</v>
+        <v>44475</v>
       </c>
       <c r="E130">
+        <f t="shared" si="0"/>
         <v>129</v>
       </c>
       <c r="O130" t="s">
         <v>153</v>
       </c>
       <c r="P130" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="Q130" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
+      <c r="A131" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="6">
         <v>43794</v>
       </c>
-      <c r="D131" s="1">
-        <v>44475</v>
-      </c>
-      <c r="E131">
+      <c r="D131" s="6">
+        <v>44651</v>
+      </c>
+      <c r="E131" s="5">
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="O131" t="s">
         <v>153</v>
       </c>
       <c r="P131" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="Q131" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A132" s="5" t="s">
+      <c r="A132" t="s">
         <v>30</v>
       </c>
-      <c r="B132" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C132" s="6">
-        <v>43794</v>
-      </c>
-      <c r="D132" s="6">
-        <v>44651</v>
-      </c>
-      <c r="E132" s="5">
+      <c r="B132" t="s">
+        <v>33</v>
+      </c>
+      <c r="C132" s="1">
+        <v>43791</v>
+      </c>
+      <c r="D132" s="1">
+        <v>43915</v>
+      </c>
+      <c r="E132">
+        <f t="shared" si="0"/>
         <v>131</v>
       </c>
+      <c r="F132">
+        <v>33.611153000000002</v>
+      </c>
+      <c r="G132">
+        <v>-111.039686</v>
+      </c>
+      <c r="H132">
+        <v>2500</v>
+      </c>
+      <c r="I132" t="s">
+        <v>15</v>
+      </c>
+      <c r="J132" t="s">
+        <v>16</v>
+      </c>
+      <c r="K132">
+        <v>417.48</v>
+      </c>
+      <c r="L132">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="M132">
+        <v>210.24299999999999</v>
+      </c>
+      <c r="N132">
+        <v>210.24299999999999</v>
+      </c>
       <c r="O132" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="P132" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="Q132" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.3">
@@ -8237,9 +8297,10 @@
         <v>43791</v>
       </c>
       <c r="D133" s="1">
-        <v>43915</v>
+        <v>44119</v>
       </c>
       <c r="E133">
+        <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="F133">
@@ -8264,19 +8325,19 @@
         <v>19.899999999999999</v>
       </c>
       <c r="M133">
-        <v>210.24299999999999</v>
+        <v>245.63200000000001</v>
       </c>
       <c r="N133">
-        <v>210.24299999999999</v>
+        <v>35.631999999999998</v>
       </c>
       <c r="O133" t="s">
         <v>154</v>
       </c>
       <c r="P133" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="Q133" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.3">
@@ -8290,46 +8351,20 @@
         <v>43791</v>
       </c>
       <c r="D134" s="1">
-        <v>44119</v>
+        <v>44287</v>
       </c>
       <c r="E134">
+        <f t="shared" si="0"/>
         <v>133</v>
-      </c>
-      <c r="F134">
-        <v>33.611153000000002</v>
-      </c>
-      <c r="G134">
-        <v>-111.039686</v>
-      </c>
-      <c r="H134">
-        <v>2500</v>
-      </c>
-      <c r="I134" t="s">
-        <v>15</v>
-      </c>
-      <c r="J134" t="s">
-        <v>16</v>
-      </c>
-      <c r="K134">
-        <v>417.48</v>
-      </c>
-      <c r="L134">
-        <v>19.899999999999999</v>
-      </c>
-      <c r="M134">
-        <v>245.63200000000001</v>
-      </c>
-      <c r="N134">
-        <v>35.631999999999998</v>
       </c>
       <c r="O134" t="s">
         <v>154</v>
       </c>
       <c r="P134" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="Q134" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.3">
@@ -8343,71 +8378,101 @@
         <v>43791</v>
       </c>
       <c r="D135" s="1">
-        <v>44287</v>
+        <v>44477</v>
       </c>
       <c r="E135">
+        <f t="shared" si="0"/>
         <v>134</v>
       </c>
       <c r="O135" t="s">
         <v>154</v>
       </c>
       <c r="P135" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="Q135" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
+      <c r="A136" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C136" s="1">
+      <c r="C136" s="6">
         <v>43791</v>
       </c>
-      <c r="D136" s="1">
-        <v>44477</v>
-      </c>
-      <c r="E136">
+      <c r="D136" s="6">
+        <v>44648</v>
+      </c>
+      <c r="E136" s="5">
+        <f t="shared" si="0"/>
         <v>135</v>
       </c>
       <c r="O136" t="s">
         <v>154</v>
       </c>
       <c r="P136" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="Q136" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A137" s="5" t="s">
+      <c r="A137" t="s">
         <v>30</v>
       </c>
-      <c r="B137" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C137" s="6">
-        <v>43791</v>
-      </c>
-      <c r="D137" s="6">
-        <v>44648</v>
-      </c>
-      <c r="E137" s="5">
+      <c r="B137" t="s">
+        <v>34</v>
+      </c>
+      <c r="C137" s="1">
+        <v>43790</v>
+      </c>
+      <c r="D137" s="1">
+        <v>43917</v>
+      </c>
+      <c r="E137">
+        <f t="shared" si="0"/>
         <v>136</v>
       </c>
+      <c r="F137">
+        <v>33.513851000000003</v>
+      </c>
+      <c r="G137">
+        <v>-111.879212</v>
+      </c>
+      <c r="H137">
+        <v>1263</v>
+      </c>
+      <c r="I137" t="s">
+        <v>16</v>
+      </c>
+      <c r="J137" t="s">
+        <v>15</v>
+      </c>
+      <c r="K137">
+        <v>245.02</v>
+      </c>
+      <c r="L137">
+        <v>22.4</v>
+      </c>
+      <c r="M137">
+        <v>172.499</v>
+      </c>
+      <c r="N137">
+        <v>172.499</v>
+      </c>
       <c r="O137" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="P137" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="Q137" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.3">
@@ -8421,9 +8486,10 @@
         <v>43790</v>
       </c>
       <c r="D138" s="1">
-        <v>43917</v>
+        <v>44117</v>
       </c>
       <c r="E138">
+        <f t="shared" si="0"/>
         <v>137</v>
       </c>
       <c r="F138">
@@ -8448,19 +8514,19 @@
         <v>22.4</v>
       </c>
       <c r="M138">
-        <v>172.499</v>
+        <v>186.459</v>
       </c>
       <c r="N138">
-        <v>172.499</v>
+        <v>13.959</v>
       </c>
       <c r="O138" t="s">
         <v>155</v>
       </c>
       <c r="P138" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="Q138" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.3">
@@ -8474,98 +8540,101 @@
         <v>43790</v>
       </c>
       <c r="D139" s="1">
-        <v>44117</v>
+        <v>44286</v>
       </c>
       <c r="E139">
+        <f t="shared" si="0"/>
         <v>138</v>
-      </c>
-      <c r="F139">
-        <v>33.513851000000003</v>
-      </c>
-      <c r="G139">
-        <v>-111.879212</v>
-      </c>
-      <c r="H139">
-        <v>1263</v>
-      </c>
-      <c r="I139" t="s">
-        <v>16</v>
-      </c>
-      <c r="J139" t="s">
-        <v>15</v>
-      </c>
-      <c r="K139">
-        <v>245.02</v>
-      </c>
-      <c r="L139">
-        <v>22.4</v>
-      </c>
-      <c r="M139">
-        <v>186.459</v>
-      </c>
-      <c r="N139">
-        <v>13.959</v>
       </c>
       <c r="O139" t="s">
         <v>155</v>
       </c>
       <c r="P139" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="Q139" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
+      <c r="A140" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C140" s="1">
+      <c r="C140" s="6">
         <v>43790</v>
       </c>
-      <c r="D140" s="1">
-        <v>44286</v>
-      </c>
-      <c r="E140">
+      <c r="D140" s="6">
+        <v>44482</v>
+      </c>
+      <c r="E140" s="5">
+        <f t="shared" si="0"/>
         <v>139</v>
       </c>
       <c r="O140" t="s">
         <v>155</v>
       </c>
       <c r="P140" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="Q140" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A141" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B141" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C141" s="6">
-        <v>43790</v>
-      </c>
-      <c r="D141" s="6">
-        <v>44482</v>
-      </c>
-      <c r="E141" s="5">
+      <c r="A141" t="s">
+        <v>35</v>
+      </c>
+      <c r="B141" t="s">
+        <v>36</v>
+      </c>
+      <c r="C141" s="1">
+        <v>43686</v>
+      </c>
+      <c r="D141" s="1">
+        <v>43781</v>
+      </c>
+      <c r="E141">
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
+      <c r="F141">
+        <v>31.58323</v>
+      </c>
+      <c r="G141">
+        <v>-110.735</v>
+      </c>
+      <c r="H141">
+        <v>4331</v>
+      </c>
+      <c r="I141" t="s">
+        <v>15</v>
+      </c>
+      <c r="J141" t="s">
+        <v>16</v>
+      </c>
+      <c r="K141">
+        <v>485.89</v>
+      </c>
+      <c r="L141">
+        <v>16.5</v>
+      </c>
+      <c r="M141">
+        <v>50.36</v>
+      </c>
+      <c r="N141">
+        <v>50.36</v>
+      </c>
       <c r="O141" t="s">
-        <v>155</v>
-      </c>
-      <c r="P141" t="s">
-        <v>317</v>
-      </c>
-      <c r="Q141" t="s">
-        <v>318</v>
+        <v>156</v>
+      </c>
+      <c r="P141" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q141" s="4" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.3">
@@ -8579,9 +8648,10 @@
         <v>43686</v>
       </c>
       <c r="D142" s="1">
-        <v>43781</v>
+        <v>43920</v>
       </c>
       <c r="E142">
+        <f t="shared" si="0"/>
         <v>141</v>
       </c>
       <c r="F142">
@@ -8606,19 +8676,19 @@
         <v>16.5</v>
       </c>
       <c r="M142">
-        <v>50.36</v>
+        <v>381.99099999999999</v>
       </c>
       <c r="N142">
-        <v>50.36</v>
+        <v>331.59100000000001</v>
       </c>
       <c r="O142" t="s">
         <v>156</v>
       </c>
       <c r="P142" s="4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="Q142" s="4" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.3">
@@ -8632,9 +8702,10 @@
         <v>43686</v>
       </c>
       <c r="D143" s="1">
-        <v>43920</v>
+        <v>44105</v>
       </c>
       <c r="E143">
+        <f t="shared" si="0"/>
         <v>142</v>
       </c>
       <c r="F143">
@@ -8659,19 +8730,19 @@
         <v>16.5</v>
       </c>
       <c r="M143">
-        <v>381.99099999999999</v>
+        <v>429.62900000000002</v>
       </c>
       <c r="N143">
-        <v>331.59100000000001</v>
+        <v>48.628999999999998</v>
       </c>
       <c r="O143" t="s">
         <v>156</v>
       </c>
       <c r="P143" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="Q143" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.3">
@@ -8685,46 +8756,20 @@
         <v>43686</v>
       </c>
       <c r="D144" s="1">
-        <v>44105</v>
+        <v>44108</v>
       </c>
       <c r="E144">
+        <f t="shared" si="0"/>
         <v>143</v>
-      </c>
-      <c r="F144">
-        <v>31.58323</v>
-      </c>
-      <c r="G144">
-        <v>-110.735</v>
-      </c>
-      <c r="H144">
-        <v>4331</v>
-      </c>
-      <c r="I144" t="s">
-        <v>15</v>
-      </c>
-      <c r="J144" t="s">
-        <v>16</v>
-      </c>
-      <c r="K144">
-        <v>485.89</v>
-      </c>
-      <c r="L144">
-        <v>16.5</v>
-      </c>
-      <c r="M144">
-        <v>429.62900000000002</v>
-      </c>
-      <c r="N144">
-        <v>48.628999999999998</v>
       </c>
       <c r="O144" t="s">
         <v>156</v>
       </c>
-      <c r="P144" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="Q144" s="4" t="s">
-        <v>331</v>
+      <c r="P144" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.3">
@@ -8738,19 +8783,20 @@
         <v>43686</v>
       </c>
       <c r="D145" s="1">
-        <v>44108</v>
+        <v>44267</v>
       </c>
       <c r="E145">
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="O145" t="s">
         <v>156</v>
       </c>
       <c r="P145" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="Q145" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.3">
@@ -8764,19 +8810,20 @@
         <v>43686</v>
       </c>
       <c r="D146" s="1">
-        <v>44267</v>
+        <v>44482</v>
       </c>
       <c r="E146">
+        <f t="shared" si="0"/>
         <v>145</v>
       </c>
       <c r="O146" t="s">
         <v>156</v>
       </c>
       <c r="P146" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q146" t="s">
-        <v>333</v>
+        <v>326</v>
+      </c>
+      <c r="Q146" s="3" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.3">
@@ -8790,19 +8837,20 @@
         <v>43686</v>
       </c>
       <c r="D147" s="1">
-        <v>44482</v>
+        <v>44483</v>
       </c>
       <c r="E147">
+        <f t="shared" si="0"/>
         <v>146</v>
       </c>
       <c r="O147" t="s">
         <v>156</v>
       </c>
       <c r="P147" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="Q147" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.3">
@@ -8816,71 +8864,101 @@
         <v>43686</v>
       </c>
       <c r="D148" s="1">
-        <v>44483</v>
+        <v>44650</v>
       </c>
       <c r="E148">
+        <f t="shared" si="0"/>
         <v>147</v>
       </c>
       <c r="O148" t="s">
         <v>156</v>
       </c>
       <c r="P148" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="Q148" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
+      <c r="A149" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C149" s="1">
+      <c r="C149" s="6">
         <v>43686</v>
       </c>
-      <c r="D149" s="1">
-        <v>44650</v>
-      </c>
-      <c r="E149">
+      <c r="D149" s="6">
+        <v>44651</v>
+      </c>
+      <c r="E149" s="5">
+        <f t="shared" si="0"/>
         <v>148</v>
       </c>
       <c r="O149" t="s">
         <v>156</v>
       </c>
       <c r="P149" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="Q149" s="3" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A150" s="5" t="s">
+      <c r="A150" t="s">
         <v>35</v>
       </c>
-      <c r="B150" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C150" s="6">
+      <c r="B150" t="s">
+        <v>37</v>
+      </c>
+      <c r="C150" s="1">
         <v>43686</v>
       </c>
-      <c r="D150" s="6">
-        <v>44651</v>
-      </c>
-      <c r="E150" s="5">
+      <c r="D150" s="1">
+        <v>43776</v>
+      </c>
+      <c r="E150">
+        <f t="shared" si="0"/>
         <v>149</v>
       </c>
+      <c r="F150">
+        <v>31.786117000000001</v>
+      </c>
+      <c r="G150">
+        <v>-110.823944</v>
+      </c>
+      <c r="H150">
+        <v>3868</v>
+      </c>
+      <c r="I150" t="s">
+        <v>15</v>
+      </c>
+      <c r="J150" t="s">
+        <v>16</v>
+      </c>
+      <c r="K150">
+        <v>534.92999999999995</v>
+      </c>
+      <c r="L150">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="M150">
+        <v>139.25</v>
+      </c>
+      <c r="N150">
+        <v>139.25</v>
+      </c>
       <c r="O150" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="P150" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q150" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
+      </c>
+      <c r="Q150" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.3">
@@ -8894,9 +8972,10 @@
         <v>43686</v>
       </c>
       <c r="D151" s="1">
-        <v>43776</v>
+        <v>43923</v>
       </c>
       <c r="E151">
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="F151">
@@ -8921,19 +9000,19 @@
         <v>17.899999999999999</v>
       </c>
       <c r="M151">
-        <v>139.25</v>
+        <v>388.24</v>
       </c>
       <c r="N151">
-        <v>139.25</v>
+        <v>248.94</v>
       </c>
       <c r="O151" t="s">
         <v>157</v>
       </c>
       <c r="P151" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="Q151" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.3">
@@ -8947,9 +9026,10 @@
         <v>43686</v>
       </c>
       <c r="D152" s="1">
-        <v>43923</v>
+        <v>44104</v>
       </c>
       <c r="E152">
+        <f t="shared" si="0"/>
         <v>151</v>
       </c>
       <c r="F152">
@@ -8974,19 +9054,19 @@
         <v>17.899999999999999</v>
       </c>
       <c r="M152">
-        <v>388.24</v>
+        <v>507.71499999999997</v>
       </c>
       <c r="N152">
-        <v>248.94</v>
+        <v>119.715</v>
       </c>
       <c r="O152" t="s">
         <v>157</v>
       </c>
       <c r="P152" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="Q152" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.3">
@@ -9000,46 +9080,20 @@
         <v>43686</v>
       </c>
       <c r="D153" s="1">
-        <v>44104</v>
+        <v>44265</v>
       </c>
       <c r="E153">
+        <f t="shared" si="0"/>
         <v>152</v>
-      </c>
-      <c r="F153">
-        <v>31.786117000000001</v>
-      </c>
-      <c r="G153">
-        <v>-110.823944</v>
-      </c>
-      <c r="H153">
-        <v>3868</v>
-      </c>
-      <c r="I153" t="s">
-        <v>15</v>
-      </c>
-      <c r="J153" t="s">
-        <v>16</v>
-      </c>
-      <c r="K153">
-        <v>534.92999999999995</v>
-      </c>
-      <c r="L153">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="M153">
-        <v>507.71499999999997</v>
-      </c>
-      <c r="N153">
-        <v>119.715</v>
       </c>
       <c r="O153" t="s">
         <v>157</v>
       </c>
       <c r="P153" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="Q153" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.3">
@@ -9053,19 +9107,20 @@
         <v>43686</v>
       </c>
       <c r="D154" s="1">
-        <v>44265</v>
+        <v>44266</v>
       </c>
       <c r="E154">
+        <f t="shared" si="0"/>
         <v>153</v>
       </c>
       <c r="O154" t="s">
         <v>157</v>
       </c>
       <c r="P154" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="Q154" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.3">
@@ -9079,19 +9134,20 @@
         <v>43686</v>
       </c>
       <c r="D155" s="1">
-        <v>44266</v>
+        <v>44475</v>
       </c>
       <c r="E155">
+        <f t="shared" si="0"/>
         <v>154</v>
       </c>
       <c r="O155" t="s">
         <v>157</v>
       </c>
       <c r="P155" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q155" t="s">
-        <v>353</v>
+        <v>343</v>
+      </c>
+      <c r="Q155" s="3" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.3">
@@ -9105,19 +9161,20 @@
         <v>43686</v>
       </c>
       <c r="D156" s="1">
-        <v>44475</v>
+        <v>44476</v>
       </c>
       <c r="E156">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
       <c r="O156" t="s">
         <v>157</v>
       </c>
       <c r="P156" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Q156" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.3">
@@ -9131,19 +9188,20 @@
         <v>43686</v>
       </c>
       <c r="D157" s="1">
-        <v>44476</v>
+        <v>44477</v>
       </c>
       <c r="E157">
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="O157" t="s">
         <v>157</v>
       </c>
       <c r="P157" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="Q157" s="3" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.3">
@@ -9157,19 +9215,20 @@
         <v>43686</v>
       </c>
       <c r="D158" s="1">
-        <v>44477</v>
+        <v>44478</v>
       </c>
       <c r="E158">
+        <f t="shared" si="0"/>
         <v>157</v>
       </c>
       <c r="O158" t="s">
         <v>157</v>
       </c>
       <c r="P158" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="Q158" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.3">
@@ -9183,19 +9242,20 @@
         <v>43686</v>
       </c>
       <c r="D159" s="1">
-        <v>44478</v>
+        <v>44643</v>
       </c>
       <c r="E159">
+        <f t="shared" si="0"/>
         <v>158</v>
       </c>
       <c r="O159" t="s">
         <v>157</v>
       </c>
       <c r="P159" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="Q159" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.3">
@@ -9209,71 +9269,101 @@
         <v>43686</v>
       </c>
       <c r="D160" s="1">
-        <v>44643</v>
+        <v>44644</v>
       </c>
       <c r="E160">
+        <f t="shared" si="0"/>
         <v>159</v>
       </c>
       <c r="O160" t="s">
         <v>157</v>
       </c>
       <c r="P160" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="Q160" s="3" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+      <c r="A161" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C161" s="1">
+      <c r="C161" s="6">
         <v>43686</v>
       </c>
-      <c r="D161" s="1">
-        <v>44644</v>
-      </c>
-      <c r="E161">
+      <c r="D161" s="6">
+        <v>44648</v>
+      </c>
+      <c r="E161" s="5">
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="O161" t="s">
         <v>157</v>
       </c>
       <c r="P161" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="Q161" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A162" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C162" s="6">
-        <v>43686</v>
-      </c>
-      <c r="D162" s="6">
-        <v>44648</v>
-      </c>
-      <c r="E162" s="5">
+      <c r="A162" t="s">
+        <v>38</v>
+      </c>
+      <c r="B162" t="s">
+        <v>39</v>
+      </c>
+      <c r="C162" s="1">
+        <v>43390</v>
+      </c>
+      <c r="D162" s="1">
+        <v>43406</v>
+      </c>
+      <c r="E162">
+        <f t="shared" si="0"/>
         <v>161</v>
       </c>
+      <c r="F162">
+        <v>38.137472000000002</v>
+      </c>
+      <c r="G162">
+        <v>-109.612444</v>
+      </c>
+      <c r="H162">
+        <v>5331</v>
+      </c>
+      <c r="I162" t="s">
+        <v>16</v>
+      </c>
+      <c r="J162" t="s">
+        <v>16</v>
+      </c>
+      <c r="K162">
+        <v>224.99</v>
+      </c>
+      <c r="L162">
+        <v>12</v>
+      </c>
+      <c r="M162">
+        <v>11.888000010000001</v>
+      </c>
+      <c r="N162">
+        <v>11.888000010000001</v>
+      </c>
       <c r="O162" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="P162" t="s">
-        <v>349</v>
-      </c>
-      <c r="Q162" s="3" t="s">
-        <v>360</v>
+        <v>361</v>
+      </c>
+      <c r="Q162" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.3">
@@ -9287,9 +9377,10 @@
         <v>43390</v>
       </c>
       <c r="D163" s="1">
-        <v>43406</v>
+        <v>43420</v>
       </c>
       <c r="E163">
+        <f t="shared" si="0"/>
         <v>162</v>
       </c>
       <c r="F163">
@@ -9314,19 +9405,19 @@
         <v>12</v>
       </c>
       <c r="M163">
-        <v>11.888000010000001</v>
+        <v>13.5</v>
       </c>
       <c r="N163">
-        <v>11.888000010000001</v>
+        <v>1.6</v>
       </c>
       <c r="O163" t="s">
         <v>158</v>
       </c>
       <c r="P163" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="Q163" t="s">
-        <v>361</v>
+        <v>379</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.3">
@@ -9340,9 +9431,10 @@
         <v>43390</v>
       </c>
       <c r="D164" s="1">
-        <v>43420</v>
+        <v>43445</v>
       </c>
       <c r="E164">
+        <f t="shared" si="0"/>
         <v>163</v>
       </c>
       <c r="F164">
@@ -9367,19 +9459,19 @@
         <v>12</v>
       </c>
       <c r="M164">
-        <v>13.5</v>
+        <v>21.71999997</v>
       </c>
       <c r="N164">
-        <v>1.6</v>
+        <v>8.2199999699999999</v>
       </c>
       <c r="O164" t="s">
         <v>158</v>
       </c>
       <c r="P164" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="Q164" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.3">
@@ -9393,9 +9485,10 @@
         <v>43390</v>
       </c>
       <c r="D165" s="1">
-        <v>43445</v>
+        <v>43546</v>
       </c>
       <c r="E165">
+        <f t="shared" si="0"/>
         <v>164</v>
       </c>
       <c r="F165">
@@ -9420,19 +9513,19 @@
         <v>12</v>
       </c>
       <c r="M165">
-        <v>21.71999997</v>
+        <v>138.637</v>
       </c>
       <c r="N165">
-        <v>8.2199999699999999</v>
+        <v>116.937</v>
       </c>
       <c r="O165" t="s">
         <v>158</v>
       </c>
       <c r="P165" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="Q165" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.3">
@@ -9446,9 +9539,10 @@
         <v>43390</v>
       </c>
       <c r="D166" s="1">
-        <v>43546</v>
+        <v>43560</v>
       </c>
       <c r="E166">
+        <f t="shared" si="0"/>
         <v>165</v>
       </c>
       <c r="F166">
@@ -9473,19 +9567,19 @@
         <v>12</v>
       </c>
       <c r="M166">
-        <v>138.637</v>
+        <v>140.042</v>
       </c>
       <c r="N166">
-        <v>116.937</v>
+        <v>1.44</v>
       </c>
       <c r="O166" t="s">
         <v>158</v>
       </c>
       <c r="P166" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="Q166" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.3">
@@ -9499,9 +9593,10 @@
         <v>43390</v>
       </c>
       <c r="D167" s="1">
-        <v>43560</v>
+        <v>43580</v>
       </c>
       <c r="E167">
+        <f t="shared" si="0"/>
         <v>166</v>
       </c>
       <c r="F167">
@@ -9526,19 +9621,19 @@
         <v>12</v>
       </c>
       <c r="M167">
-        <v>140.042</v>
+        <v>144.96799999999999</v>
       </c>
       <c r="N167">
-        <v>1.44</v>
+        <v>4.968</v>
       </c>
       <c r="O167" t="s">
         <v>158</v>
       </c>
       <c r="P167" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="Q167" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="168" spans="1:17" x14ac:dyDescent="0.3">
@@ -9552,9 +9647,10 @@
         <v>43390</v>
       </c>
       <c r="D168" s="1">
-        <v>43580</v>
+        <v>43602</v>
       </c>
       <c r="E168">
+        <f t="shared" si="0"/>
         <v>167</v>
       </c>
       <c r="F168">
@@ -9579,19 +9675,19 @@
         <v>12</v>
       </c>
       <c r="M168">
-        <v>144.96799999999999</v>
+        <v>165.39899969999999</v>
       </c>
       <c r="N168">
-        <v>4.968</v>
+        <v>20.498999699999999</v>
       </c>
       <c r="O168" t="s">
         <v>158</v>
       </c>
       <c r="P168" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="Q168" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="169" spans="1:17" x14ac:dyDescent="0.3">
@@ -9605,9 +9701,10 @@
         <v>43390</v>
       </c>
       <c r="D169" s="1">
-        <v>43602</v>
+        <v>43629</v>
       </c>
       <c r="E169">
+        <f t="shared" si="0"/>
         <v>168</v>
       </c>
       <c r="F169">
@@ -9632,19 +9729,19 @@
         <v>12</v>
       </c>
       <c r="M169">
-        <v>165.39899969999999</v>
+        <v>190.71899930000001</v>
       </c>
       <c r="N169">
-        <v>20.498999699999999</v>
+        <v>25.318999300000002</v>
       </c>
       <c r="O169" t="s">
         <v>158</v>
       </c>
       <c r="P169" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="Q169" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.3">
@@ -9658,9 +9755,10 @@
         <v>43390</v>
       </c>
       <c r="D170" s="1">
-        <v>43629</v>
+        <v>43670</v>
       </c>
       <c r="E170">
+        <f t="shared" si="0"/>
         <v>169</v>
       </c>
       <c r="F170">
@@ -9685,35 +9783,36 @@
         <v>12</v>
       </c>
       <c r="M170">
-        <v>190.71899930000001</v>
+        <v>209.50099879999999</v>
       </c>
       <c r="N170">
-        <v>25.318999300000002</v>
+        <v>18.800998799999999</v>
       </c>
       <c r="O170" t="s">
         <v>158</v>
       </c>
       <c r="P170" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Q170" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
+      <c r="A171" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C171" s="1">
+      <c r="C171" s="6">
         <v>43390</v>
       </c>
-      <c r="D171" s="1">
-        <v>43670</v>
-      </c>
-      <c r="E171">
+      <c r="D171" s="6">
+        <v>44375</v>
+      </c>
+      <c r="E171" s="5">
+        <f t="shared" si="0"/>
         <v>170</v>
       </c>
       <c r="F171">
@@ -9738,72 +9837,73 @@
         <v>12</v>
       </c>
       <c r="M171">
-        <v>209.50099879999999</v>
+        <v>453.24</v>
       </c>
       <c r="N171">
-        <v>18.800998799999999</v>
+        <v>243.73900119999999</v>
       </c>
       <c r="O171" t="s">
         <v>158</v>
       </c>
-      <c r="P171" t="s">
-        <v>369</v>
-      </c>
-      <c r="Q171" t="s">
-        <v>372</v>
+      <c r="P171" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q171" s="4" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A172" s="5" t="s">
+      <c r="A172" t="s">
         <v>38</v>
       </c>
-      <c r="B172" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C172" s="6">
-        <v>43390</v>
-      </c>
-      <c r="D172" s="6">
-        <v>44375</v>
-      </c>
-      <c r="E172" s="5">
+      <c r="B172" t="s">
+        <v>40</v>
+      </c>
+      <c r="C172" s="1">
+        <v>43404</v>
+      </c>
+      <c r="D172" s="1">
+        <v>43431</v>
+      </c>
+      <c r="E172">
+        <f t="shared" si="0"/>
         <v>171</v>
       </c>
       <c r="F172">
-        <v>38.137472000000002</v>
+        <v>39.228361</v>
       </c>
       <c r="G172">
-        <v>-109.612444</v>
+        <v>-109.001389</v>
       </c>
       <c r="H172">
-        <v>5331</v>
+        <v>4724</v>
       </c>
       <c r="I172" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J172" t="s">
         <v>16</v>
       </c>
       <c r="K172">
-        <v>224.99</v>
+        <v>273.55</v>
       </c>
       <c r="L172">
         <v>12</v>
       </c>
       <c r="M172">
-        <v>453.24</v>
+        <v>0.54</v>
       </c>
       <c r="N172">
-        <v>243.73900119999999</v>
+        <v>0.54</v>
       </c>
       <c r="O172" t="s">
-        <v>158</v>
-      </c>
-      <c r="P172" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="Q172" s="4" t="s">
-        <v>371</v>
+        <v>159</v>
+      </c>
+      <c r="P172" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q172" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.3">
@@ -9817,9 +9917,10 @@
         <v>43404</v>
       </c>
       <c r="D173" s="1">
-        <v>43431</v>
+        <v>43446</v>
       </c>
       <c r="E173">
+        <f t="shared" si="0"/>
         <v>172</v>
       </c>
       <c r="F173">
@@ -9844,19 +9945,19 @@
         <v>12</v>
       </c>
       <c r="M173">
-        <v>0.54</v>
+        <v>8.57</v>
       </c>
       <c r="N173">
-        <v>0.54</v>
+        <v>8.07</v>
       </c>
       <c r="O173" t="s">
         <v>159</v>
       </c>
       <c r="P173" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="Q173" t="s">
-        <v>380</v>
+        <v>396</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.3">
@@ -9870,9 +9971,10 @@
         <v>43404</v>
       </c>
       <c r="D174" s="1">
-        <v>43446</v>
+        <v>43553</v>
       </c>
       <c r="E174">
+        <f t="shared" si="0"/>
         <v>173</v>
       </c>
       <c r="F174">
@@ -9897,19 +9999,19 @@
         <v>12</v>
       </c>
       <c r="M174">
-        <v>8.57</v>
+        <v>139.24600000000001</v>
       </c>
       <c r="N174">
-        <v>8.07</v>
+        <v>130.64599999999999</v>
       </c>
       <c r="O174" t="s">
         <v>159</v>
       </c>
       <c r="P174" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="Q174" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.3">
@@ -9923,9 +10025,10 @@
         <v>43404</v>
       </c>
       <c r="D175" s="1">
-        <v>43553</v>
+        <v>43574</v>
       </c>
       <c r="E175">
+        <f t="shared" si="0"/>
         <v>174</v>
       </c>
       <c r="F175">
@@ -9950,19 +10053,19 @@
         <v>12</v>
       </c>
       <c r="M175">
-        <v>139.24600000000001</v>
+        <v>141.42500000000001</v>
       </c>
       <c r="N175">
-        <v>130.64599999999999</v>
+        <v>2.4249999999999998</v>
       </c>
       <c r="O175" t="s">
         <v>159</v>
       </c>
       <c r="P175" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="Q175" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.3">
@@ -9976,9 +10079,10 @@
         <v>43404</v>
       </c>
       <c r="D176" s="1">
-        <v>43574</v>
+        <v>43594</v>
       </c>
       <c r="E176">
+        <f t="shared" si="0"/>
         <v>175</v>
       </c>
       <c r="F176">
@@ -10003,19 +10107,19 @@
         <v>12</v>
       </c>
       <c r="M176">
-        <v>141.42500000000001</v>
+        <v>177.232</v>
       </c>
       <c r="N176">
-        <v>2.4249999999999998</v>
+        <v>35.832000000000001</v>
       </c>
       <c r="O176" t="s">
         <v>159</v>
       </c>
       <c r="P176" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="Q176" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.3">
@@ -10029,9 +10133,10 @@
         <v>43404</v>
       </c>
       <c r="D177" s="1">
-        <v>43594</v>
+        <v>43613</v>
       </c>
       <c r="E177">
+        <f t="shared" si="0"/>
         <v>176</v>
       </c>
       <c r="F177">
@@ -10059,16 +10164,16 @@
         <v>177.232</v>
       </c>
       <c r="N177">
-        <v>35.832000000000001</v>
+        <v>0</v>
       </c>
       <c r="O177" t="s">
         <v>159</v>
       </c>
       <c r="P177" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="Q177" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.3">
@@ -10082,9 +10187,10 @@
         <v>43404</v>
       </c>
       <c r="D178" s="1">
-        <v>43613</v>
+        <v>43647</v>
       </c>
       <c r="E178">
+        <f t="shared" si="0"/>
         <v>177</v>
       </c>
       <c r="F178">
@@ -10109,19 +10215,19 @@
         <v>12</v>
       </c>
       <c r="M178">
-        <v>177.232</v>
+        <v>222.52</v>
       </c>
       <c r="N178">
-        <v>0</v>
+        <v>45.52</v>
       </c>
       <c r="O178" t="s">
         <v>159</v>
       </c>
       <c r="P178" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="Q178" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.3">
@@ -10135,9 +10241,10 @@
         <v>43404</v>
       </c>
       <c r="D179" s="1">
-        <v>43647</v>
+        <v>43684</v>
       </c>
       <c r="E179">
+        <f t="shared" si="0"/>
         <v>178</v>
       </c>
       <c r="F179">
@@ -10162,35 +10269,36 @@
         <v>12</v>
       </c>
       <c r="M179">
-        <v>222.52</v>
+        <v>242.953</v>
       </c>
       <c r="N179">
-        <v>45.52</v>
+        <v>20.452999999999999</v>
       </c>
       <c r="O179" t="s">
         <v>159</v>
       </c>
       <c r="P179" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="Q179" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
+      <c r="A180" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C180" s="1">
+      <c r="C180" s="6">
         <v>43404</v>
       </c>
-      <c r="D180" s="1">
-        <v>43684</v>
-      </c>
-      <c r="E180">
+      <c r="D180" s="6">
+        <v>44376</v>
+      </c>
+      <c r="E180" s="5">
+        <f t="shared" si="0"/>
         <v>179</v>
       </c>
       <c r="F180">
@@ -10215,45 +10323,46 @@
         <v>12</v>
       </c>
       <c r="M180">
-        <v>242.953</v>
+        <v>374.18299999999999</v>
       </c>
       <c r="N180">
-        <v>20.452999999999999</v>
+        <v>131.22999999999999</v>
       </c>
       <c r="O180" t="s">
         <v>159</v>
       </c>
-      <c r="P180" t="s">
-        <v>387</v>
-      </c>
-      <c r="Q180" t="s">
-        <v>390</v>
+      <c r="P180" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q180" s="4" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A181" s="5" t="s">
+      <c r="A181" t="s">
         <v>38</v>
       </c>
-      <c r="B181" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C181" s="6">
-        <v>43404</v>
-      </c>
-      <c r="D181" s="6">
-        <v>44376</v>
-      </c>
-      <c r="E181" s="5">
+      <c r="B181" t="s">
+        <v>41</v>
+      </c>
+      <c r="C181" s="1">
+        <v>43402</v>
+      </c>
+      <c r="D181" s="1">
+        <v>43420</v>
+      </c>
+      <c r="E181">
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
       <c r="F181">
-        <v>39.228361</v>
+        <v>38.29448</v>
       </c>
       <c r="G181">
-        <v>-109.001389</v>
+        <v>-109.06452</v>
       </c>
       <c r="H181">
-        <v>4724</v>
+        <v>7486</v>
       </c>
       <c r="I181" t="s">
         <v>15</v>
@@ -10262,25 +10371,25 @@
         <v>16</v>
       </c>
       <c r="K181">
-        <v>273.55</v>
+        <v>415.66</v>
       </c>
       <c r="L181">
-        <v>12</v>
+        <v>8.5</v>
       </c>
       <c r="M181">
-        <v>374.18299999999999</v>
+        <v>3.38</v>
       </c>
       <c r="N181">
-        <v>131.22999999999999</v>
+        <v>3.38</v>
       </c>
       <c r="O181" t="s">
-        <v>159</v>
-      </c>
-      <c r="P181" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="Q181" s="4" t="s">
-        <v>389</v>
+        <v>160</v>
+      </c>
+      <c r="P181" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q181" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.3">
@@ -10294,9 +10403,10 @@
         <v>43402</v>
       </c>
       <c r="D182" s="1">
-        <v>43420</v>
+        <v>43432</v>
       </c>
       <c r="E182">
+        <f t="shared" ref="E182:E188" si="1">E181+1</f>
         <v>181</v>
       </c>
       <c r="F182">
@@ -10330,10 +10440,10 @@
         <v>160</v>
       </c>
       <c r="P182" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="Q182" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.3">
@@ -10347,9 +10457,10 @@
         <v>43402</v>
       </c>
       <c r="D183" s="1">
-        <v>43432</v>
+        <v>43581</v>
       </c>
       <c r="E183">
+        <f t="shared" si="1"/>
         <v>182</v>
       </c>
       <c r="F183">
@@ -10374,19 +10485,19 @@
         <v>8.5</v>
       </c>
       <c r="M183">
-        <v>3.38</v>
+        <v>209.25200000000001</v>
       </c>
       <c r="N183">
-        <v>3.38</v>
+        <v>205.75200000000001</v>
       </c>
       <c r="O183" t="s">
         <v>160</v>
       </c>
       <c r="P183" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="Q183" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.3">
@@ -10400,9 +10511,10 @@
         <v>43402</v>
       </c>
       <c r="D184" s="1">
-        <v>43581</v>
+        <v>43601</v>
       </c>
       <c r="E184">
+        <f t="shared" si="1"/>
         <v>183</v>
       </c>
       <c r="F184">
@@ -10427,19 +10539,19 @@
         <v>8.5</v>
       </c>
       <c r="M184">
-        <v>209.25200000000001</v>
+        <v>243.12200000000001</v>
       </c>
       <c r="N184">
-        <v>205.75200000000001</v>
+        <v>0</v>
       </c>
       <c r="O184" t="s">
         <v>160</v>
       </c>
       <c r="P184" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="Q184" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.3">
@@ -10453,9 +10565,10 @@
         <v>43402</v>
       </c>
       <c r="D185" s="1">
-        <v>43601</v>
+        <v>43614</v>
       </c>
       <c r="E185">
+        <f t="shared" si="1"/>
         <v>184</v>
       </c>
       <c r="F185">
@@ -10480,19 +10593,19 @@
         <v>8.5</v>
       </c>
       <c r="M185">
-        <v>243.12200000000001</v>
+        <v>284.96600000000001</v>
       </c>
       <c r="N185">
-        <v>0</v>
+        <v>41.966000000000001</v>
       </c>
       <c r="O185" t="s">
         <v>160</v>
       </c>
       <c r="P185" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="Q185" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.3">
@@ -10506,9 +10619,10 @@
         <v>43402</v>
       </c>
       <c r="D186" s="1">
-        <v>43614</v>
+        <v>43648</v>
       </c>
       <c r="E186">
+        <f t="shared" si="1"/>
         <v>185</v>
       </c>
       <c r="F186">
@@ -10533,19 +10647,19 @@
         <v>8.5</v>
       </c>
       <c r="M186">
-        <v>284.96600000000001</v>
+        <v>296.56599999999997</v>
       </c>
       <c r="N186">
-        <v>41.966000000000001</v>
+        <v>11.666</v>
       </c>
       <c r="O186" t="s">
         <v>160</v>
       </c>
       <c r="P186" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="Q186" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="187" spans="1:17" x14ac:dyDescent="0.3">
@@ -10559,9 +10673,10 @@
         <v>43402</v>
       </c>
       <c r="D187" s="1">
-        <v>43648</v>
+        <v>43683</v>
       </c>
       <c r="E187">
+        <f t="shared" si="1"/>
         <v>186</v>
       </c>
       <c r="F187">
@@ -10586,35 +10701,36 @@
         <v>8.5</v>
       </c>
       <c r="M187">
-        <v>296.56599999999997</v>
+        <v>335.43099999999998</v>
       </c>
       <c r="N187">
-        <v>11.666</v>
+        <v>38.831000000000003</v>
       </c>
       <c r="O187" t="s">
         <v>160</v>
       </c>
       <c r="P187" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="Q187" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="188" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
+      <c r="A188" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C188" s="1">
+      <c r="C188" s="6">
         <v>43402</v>
       </c>
-      <c r="D188" s="1">
-        <v>43683</v>
-      </c>
-      <c r="E188">
+      <c r="D188" s="6">
+        <v>44376</v>
+      </c>
+      <c r="E188" s="5">
+        <f t="shared" si="1"/>
         <v>187</v>
       </c>
       <c r="F188">
@@ -10639,72 +10755,43 @@
         <v>8.5</v>
       </c>
       <c r="M188">
-        <v>335.43099999999998</v>
+        <v>739.32</v>
       </c>
       <c r="N188">
-        <v>38.831000000000003</v>
+        <v>403.88900000000001</v>
       </c>
       <c r="O188" t="s">
         <v>160</v>
       </c>
-      <c r="P188" t="s">
-        <v>403</v>
+      <c r="P188" s="4" t="s">
+        <v>404</v>
       </c>
       <c r="Q188" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C189" s="6">
-        <v>43402</v>
+        <v>43903</v>
       </c>
       <c r="D189" s="6">
-        <v>44376</v>
-      </c>
-      <c r="E189" s="5">
-        <v>188</v>
-      </c>
-      <c r="F189">
-        <v>38.29448</v>
-      </c>
-      <c r="G189">
-        <v>-109.06452</v>
-      </c>
-      <c r="H189">
-        <v>7486</v>
-      </c>
-      <c r="I189" t="s">
-        <v>15</v>
-      </c>
-      <c r="J189" t="s">
-        <v>16</v>
-      </c>
-      <c r="K189">
-        <v>415.66</v>
-      </c>
-      <c r="L189">
-        <v>8.5</v>
-      </c>
-      <c r="M189">
-        <v>739.32</v>
-      </c>
-      <c r="N189">
-        <v>403.88900000000001</v>
-      </c>
+        <v>44666</v>
+      </c>
+      <c r="E189" s="5"/>
       <c r="O189" t="s">
-        <v>160</v>
-      </c>
-      <c r="P189" s="4" t="s">
-        <v>404</v>
+        <v>150</v>
+      </c>
+      <c r="P189" t="s">
+        <v>274</v>
       </c>
       <c r="Q189" t="s">
-        <v>405</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch glms to glmmTMB package
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/03.2_monitoring-events-with-Farrell-climate-data-and-PRISM-csv-file-name.xlsx
+++ b/data/data-wrangling-intermediate/03.2_monitoring-events-with-Farrell-climate-data-and-PRISM-csv-file-name.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1384,7 +1384,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1398,12 +1398,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1970,10 +1964,10 @@
   <dimension ref="A1:Q189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="L158" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E189" sqref="E189"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>